<commit_message>
added command - change remote repo url
</commit_message>
<xml_diff>
--- a/git_demo.xlsx
+++ b/git_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\githubpages\git_demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F61407-AD25-4589-AD1F-F805D5B7B553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F8E8F4-F413-462B-9744-2248FE642CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="276">
   <si>
     <t>git init</t>
   </si>
@@ -1111,6 +1111,27 @@
   </si>
   <si>
     <t>VCS &gt; Git &gt; Reset HEAD... &gt; Select previous commit, Uncommitted Changes &gt; Rollback</t>
+  </si>
+  <si>
+    <t>Rename remote repo alias</t>
+  </si>
+  <si>
+    <t>git remote rename origin gitlab</t>
+  </si>
+  <si>
+    <t>git remote rename &lt;old alias&gt; &lt;new alias&gt;</t>
+  </si>
+  <si>
+    <t>Git &gt; Manage Remotes &gt; Select Remote &gt; Edit</t>
+  </si>
+  <si>
+    <t>Change remote repo url</t>
+  </si>
+  <si>
+    <t>git remote set-url &lt;remote_name&gt; &lt;new_url&gt;</t>
+  </si>
+  <si>
+    <t>git remote set-url &lt;remote alias&gt; &lt;new  remote url&gt;</t>
   </si>
 </sst>
 </file>
@@ -1490,11 +1511,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED47341-9BD1-431D-9D81-91008CC24AF2}">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1630,15 +1651,17 @@
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="4" t="s">
-        <v>20</v>
+        <v>269</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>21</v>
+        <v>270</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="4"/>
+        <v>272</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="7">
@@ -1646,15 +1669,17 @@
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>273</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>24</v>
+        <v>274</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="4"/>
+        <v>272</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="7">
@@ -1662,13 +1687,13 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F10" s="4"/>
     </row>
@@ -1678,13 +1703,13 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F11" s="4"/>
     </row>
@@ -1694,13 +1719,13 @@
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -1710,13 +1735,13 @@
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>242</v>
+        <v>29</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>222</v>
+        <v>30</v>
       </c>
       <c r="F13" s="4"/>
     </row>
@@ -1726,13 +1751,13 @@
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>223</v>
+        <v>33</v>
       </c>
       <c r="F14" s="4"/>
     </row>
@@ -1742,13 +1767,13 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>38</v>
+        <v>242</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F15" s="4"/>
     </row>
@@ -1758,17 +1783,15 @@
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="4" t="s">
-        <v>228</v>
+        <v>35</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>233</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="7">
@@ -1776,13 +1799,13 @@
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="4" t="s">
-        <v>224</v>
+        <v>37</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>227</v>
+        <v>38</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F17" s="4"/>
     </row>
@@ -1792,15 +1815,17 @@
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="4" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>236</v>
+        <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="F18" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="7">
@@ -1808,12 +1833,14 @@
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="4" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="E19" s="4"/>
+        <v>227</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>234</v>
+      </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6">
@@ -1822,12 +1849,14 @@
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E20" s="4"/>
+        <v>236</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>237</v>
+      </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6">
@@ -1836,14 +1865,12 @@
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="4" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>231</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6">
@@ -1852,14 +1879,12 @@
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="4" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>232</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6">
@@ -1868,13 +1893,13 @@
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="4" t="s">
-        <v>41</v>
+        <v>225</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>42</v>
+        <v>229</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
       <c r="F23" s="4"/>
     </row>
@@ -1884,11 +1909,13 @@
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="5"/>
+        <v>226</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>230</v>
+      </c>
       <c r="E24" s="4" t="s">
-        <v>45</v>
+        <v>232</v>
       </c>
       <c r="F24" s="4"/>
     </row>
@@ -1898,17 +1925,15 @@
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>189</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7">
@@ -1916,13 +1941,11 @@
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D26" s="5"/>
       <c r="E26" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F26" s="4"/>
     </row>
@@ -1932,15 +1955,17 @@
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>179</v>
+        <v>46</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="7">
@@ -1948,17 +1973,15 @@
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>260</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="7">
@@ -1966,17 +1989,15 @@
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="4" t="s">
-        <v>244</v>
+        <v>52</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>56</v>
+        <v>179</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>260</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7">
@@ -1984,13 +2005,13 @@
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>260</v>
@@ -2002,13 +2023,13 @@
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>260</v>
@@ -2020,13 +2041,13 @@
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>180</v>
+        <v>58</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>248</v>
+        <v>59</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>260</v>
@@ -2038,16 +2059,16 @@
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="4" t="s">
-        <v>62</v>
+        <v>246</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>267</v>
+        <v>61</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2056,16 +2077,16 @@
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="4" t="s">
-        <v>63</v>
+        <v>247</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2074,10 +2095,10 @@
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>267</v>
@@ -2092,10 +2113,10 @@
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>267</v>
@@ -2110,10 +2131,10 @@
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>267</v>
@@ -2128,16 +2149,16 @@
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>68</v>
+        <v>184</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>186</v>
+        <v>267</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2146,16 +2167,16 @@
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>249</v>
+        <v>185</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>70</v>
+        <v>267</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2164,16 +2185,16 @@
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>250</v>
+        <v>68</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2182,16 +2203,16 @@
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>74</v>
+        <v>249</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2200,16 +2221,16 @@
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2218,16 +2239,16 @@
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>252</v>
+        <v>74</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2236,13 +2257,13 @@
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>260</v>
@@ -2254,13 +2275,13 @@
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>260</v>
@@ -2272,13 +2293,13 @@
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>260</v>
@@ -2290,16 +2311,16 @@
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>268</v>
+        <v>83</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2308,16 +2329,16 @@
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>268</v>
+        <v>85</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2326,16 +2347,16 @@
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>268</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2344,10 +2365,10 @@
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>268</v>
@@ -2362,7 +2383,7 @@
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>258</v>
@@ -2371,7 +2392,7 @@
         <v>268</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2379,17 +2400,17 @@
         <v>51</v>
       </c>
       <c r="B52" s="7"/>
-      <c r="C52" s="6" t="s">
-        <v>91</v>
+      <c r="C52" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>92</v>
+        <v>259</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>93</v>
+        <v>268</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>190</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2398,16 +2419,16 @@
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>95</v>
+        <v>258</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>96</v>
+        <v>268</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>191</v>
+        <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2415,17 +2436,17 @@
         <v>53</v>
       </c>
       <c r="B54" s="7"/>
-      <c r="C54" s="4" t="s">
-        <v>97</v>
+      <c r="C54" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2434,16 +2455,16 @@
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2452,16 +2473,16 @@
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2470,16 +2491,16 @@
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2488,16 +2509,16 @@
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2506,16 +2527,16 @@
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2524,16 +2545,16 @@
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2542,16 +2563,16 @@
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2560,16 +2581,16 @@
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2578,16 +2599,16 @@
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2596,16 +2617,16 @@
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2614,16 +2635,16 @@
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2632,16 +2653,16 @@
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2650,16 +2671,16 @@
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2668,16 +2689,16 @@
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>138</v>
+        <v>131</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2686,16 +2707,16 @@
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2704,16 +2725,16 @@
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>187</v>
+        <v>137</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2722,16 +2743,16 @@
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2740,16 +2761,16 @@
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2758,16 +2779,16 @@
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2776,16 +2797,16 @@
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2794,16 +2815,16 @@
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2812,16 +2833,16 @@
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2830,16 +2851,16 @@
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2848,16 +2869,16 @@
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2866,16 +2887,16 @@
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>163</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2884,16 +2905,16 @@
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2902,23 +2923,53 @@
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="7">
+        <v>81</v>
+      </c>
+      <c r="B82" s="7"/>
+      <c r="C82" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="7">
+        <v>82</v>
+      </c>
+      <c r="B83" s="7"/>
+      <c r="C83" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D83" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E83" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F81" s="4" t="s">
+      <c r="F83" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="F82" s="2"/>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6">
       <c r="F84" s="2"/>
@@ -2988,6 +3039,12 @@
     </row>
     <row r="106" spans="6:6">
       <c r="F106" s="2"/>
+    </row>
+    <row r="107" spans="6:6">
+      <c r="F107" s="2"/>
+    </row>
+    <row r="108" spans="6:6">
+      <c r="F108" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>